<commit_message>
generar factura pdf sponsors y calcular precio a las carreras que patrocina
</commit_message>
<xml_diff>
--- a/PlaTreball.xlsx
+++ b/PlaTreball.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t xml:space="preserve">PLA DE TREBALL</t>
   </si>
@@ -174,6 +174,15 @@
     <t xml:space="preserve">Crear relación many to many en modelos, listar para carreras
 Los patrocinadores activos, listar en la edición de
 Patrocinadores todos las carreras ordenadas por activa o no.Alexander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar pdf factura sponsor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar pdf en base a cursas activas no finalizadas del sponsor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleksandr</t>
   </si>
   <si>
     <t xml:space="preserve">Total hores estimades acumulades</t>
@@ -205,16 +214,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
@@ -794,7 +806,7 @@
     <cellStyle name="Hyperlink 15" xfId="31"/>
     <cellStyle name="Note 16" xfId="32"/>
     <cellStyle name="Result 17" xfId="33"/>
-    <cellStyle name="Result2" xfId="34"/>
+    <cellStyle name="Результат2" xfId="34"/>
     <cellStyle name="Status 18" xfId="35"/>
     <cellStyle name="Text 19" xfId="36"/>
     <cellStyle name="Warning 20" xfId="37"/>
@@ -873,9 +885,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>931680</xdr:colOff>
+      <xdr:colOff>931320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>723600</xdr:rowOff>
+      <xdr:rowOff>723240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -889,7 +901,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2403720" cy="723600"/>
+          <a:ext cx="2402280" cy="723240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -905,20 +917,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.54"/>
@@ -1221,20 +1233,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="B21" s="28"/>
+      <c r="B21" s="28" t="n">
+        <v>2</v>
+      </c>
       <c r="C21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="29"/>
+      <c r="D21" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="29" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="n">
@@ -1268,25 +1294,25 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="33"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="32" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B29" s="32" t="n">
         <f aca="false">SUM(I16:I23)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,7 +1325,7 @@
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" display="alexanderbkl/bikeroll (github.com)"/>
+    <hyperlink ref="D6" r:id="rId1" display="alexanderbkl/bikeroll (github.com) "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
@@ -1313,7 +1339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1323,7 +1349,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
@@ -1336,7 +1362,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1346,7 +1372,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>

</xml_diff>

<commit_message>
add users and pro role
</commit_message>
<xml_diff>
--- a/PlaTreball.xlsx
+++ b/PlaTreball.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t xml:space="preserve">PLA DE TREBALL</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t xml:space="preserve">La durada total de les tasques, ha de coincidir amb el nombre d'hores totals disponibles, a cada Sprint, multiplicat pel nombre d'alumnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User password admin:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin@mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adminadmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User password user:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user@mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">useruser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User password pro:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pro@mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Número d'activitat</t>
@@ -202,7 +226,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-403];[RED]\-#,##0.00\ [$€-403]"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -335,6 +359,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -630,24 +662,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,7 +788,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -764,15 +800,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -806,10 +842,10 @@
     <cellStyle name="Hyperlink 15" xfId="31"/>
     <cellStyle name="Note 16" xfId="32"/>
     <cellStyle name="Result 17" xfId="33"/>
-    <cellStyle name="Результат2" xfId="34"/>
-    <cellStyle name="Status 18" xfId="35"/>
-    <cellStyle name="Text 19" xfId="36"/>
-    <cellStyle name="Warning 20" xfId="37"/>
+    <cellStyle name="Status 18" xfId="34"/>
+    <cellStyle name="Text 19" xfId="35"/>
+    <cellStyle name="Warning 20" xfId="36"/>
+    <cellStyle name="Результат2" xfId="37"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -885,9 +921,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>931320</xdr:colOff>
+      <xdr:colOff>930960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>723240</xdr:rowOff>
+      <xdr:rowOff>722880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -901,7 +937,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="0"/>
-          <a:ext cx="2402280" cy="723240"/>
+          <a:ext cx="2402280" cy="722880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -924,10 +960,10 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -1059,264 +1095,297 @@
       <c r="E12" s="25"/>
       <c r="F12" s="26"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="27" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="30" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="B20" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="29" t="n">
+        <v>5</v>
+      </c>
+      <c r="B21" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="30" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="29" t="n">
+        <v>7</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="30"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="29" t="n">
+        <v>8</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="30"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="33" t="n">
+        <f aca="false">SUM(I17:I24)</f>
         <v>26</v>
       </c>
-      <c r="H15" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="29" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="29" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="29" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="n">
-        <v>4</v>
-      </c>
-      <c r="B19" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="29" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="29" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="n">
-        <v>6</v>
-      </c>
-      <c r="B21" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="29" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="n">
-        <v>7</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="29"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="29"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28" t="n">
-        <v>8</v>
-      </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="29"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="33"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="32" t="n">
-        <f aca="false">SUM(I16:I23)</f>
-        <v>26</v>
-      </c>
     </row>
     <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1048576" s="28" t="s">
+      <c r="C1048576" s="29" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1326,6 +1395,9 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" display="alexanderbkl/bikeroll (github.com) "/>
+    <hyperlink ref="B13" r:id="rId2" display="admin@mail.com"/>
+    <hyperlink ref="B14" r:id="rId3" display="user@mail.com"/>
+    <hyperlink ref="B15" r:id="rId4" display="pro@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
@@ -1334,7 +1406,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPàgina &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1349,7 +1421,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
@@ -1372,7 +1444,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>

</xml_diff>

<commit_message>
actualizar pla dea treball
</commit_message>
<xml_diff>
--- a/PlaTreball.xlsx
+++ b/PlaTreball.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
   <si>
     <t xml:space="preserve">PLA DE TREBALL</t>
   </si>
@@ -163,6 +163,9 @@
     <t xml:space="preserve">3 horas</t>
   </si>
   <si>
+    <t xml:space="preserve">1, 2, 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crear repositorio, modelos, 
 Controladores, migrations con relaciones
 Y tablas dinamicas Para admin</t>
@@ -177,6 +180,9 @@
     <t xml:space="preserve">Alta</t>
   </si>
   <si>
+    <t xml:space="preserve">4, 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Listar imagenes, eliminar imagenes,
 Para cada objeto, de manera
 Recíproca.</t>
@@ -189,10 +195,11 @@
     <t xml:space="preserve">3h</t>
   </si>
   <si>
+    <t xml:space="preserve">3, 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implementar relación manyToMany
-En modelo y migration (fue complicado
-Hacerlo de manera adecuada, pero
-Lo logré)</t>
+En MODELO y MIGRATION</t>
   </si>
   <si>
     <t xml:space="preserve">Crear relación many to many en modelos, listar para carreras
@@ -222,7 +229,7 @@
   </si>
   <si>
     <t xml:space="preserve">PRO introducen núm. Federación, normales seleccionan
-El seguro</t>
+El seguro, genera PDF</t>
   </si>
   <si>
     <t xml:space="preserve">2h</t>
@@ -721,7 +728,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -859,6 +866,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1009,8 +1020,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1209,7 +1220,7 @@
     </row>
     <row r="17" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" s="30" t="n">
         <v>1</v>
@@ -1238,7 +1249,7 @@
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B18" s="30" t="n">
         <v>1</v>
@@ -1266,8 +1277,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30" t="n">
-        <v>3</v>
+      <c r="A19" s="30" t="s">
+        <v>45</v>
       </c>
       <c r="B19" s="30" t="n">
         <v>1</v>
@@ -1276,27 +1287,27 @@
         <v>11</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I19" s="31" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="n">
-        <v>4</v>
+      <c r="A20" s="30" t="s">
+        <v>50</v>
       </c>
       <c r="B20" s="30" t="n">
         <v>1</v>
@@ -1305,27 +1316,27 @@
         <v>11</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>11</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I20" s="31" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="n">
-        <v>5</v>
+      <c r="A21" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="B21" s="30" t="n">
         <v>1</v>
@@ -1334,10 +1345,10 @@
         <v>11</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F21" s="31" t="s">
         <v>11</v>
@@ -1354,25 +1365,25 @@
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B22" s="30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H22" s="33" t="s">
         <v>41</v>
@@ -1383,7 +1394,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B23" s="30" t="n">
         <v>2</v>
@@ -1392,19 +1403,19 @@
         <v>11</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I23" s="31" t="n">
         <v>1</v>
@@ -1421,27 +1432,27 @@
         <v>11</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I24" s="31" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>9</v>
+      <c r="A25" s="35" t="n">
+        <v>1</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>2</v>
@@ -1450,42 +1461,48 @@
         <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>2</v>
@@ -1494,36 +1511,36 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
       <c r="B27" s="0"/>
-      <c r="C27" s="35"/>
+      <c r="C27" s="36"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="0"/>
-      <c r="C28" s="35"/>
+      <c r="C28" s="36"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="36"/>
+      <c r="A30" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="37"/>
       <c r="C30" s="0"/>
       <c r="D30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="36"/>
+      <c r="A31" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="37"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="36" t="n">
+      <c r="A32" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="37" t="n">
         <f aca="false">SUM(I17:I200)</f>
         <v>42</v>
       </c>

</xml_diff>